<commit_message>
Fetched inputs from excel for login only
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t xml:space="preserve">email</t>
   </si>
@@ -39,6 +39,48 @@
   </si>
   <si>
     <t xml:space="preserve">Login Successful</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ortu@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unexpected alert open: {Alert text : Login failed. Email not found.}
+  (Session info: chrome=136.0.7103.114): Login failed. Email not found.
+Build info: version: '4.30.0', revision: '509c7f17cc*'
+System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '23.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Command: [468adb5a54026f1a1c1dbb1d5fa1d171, getCurrentUrl {}]
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 136.0.7103.114, chrome: {chromedriverVersion: 136.0.7103.94 (fa0be0b33deb..., userDataDir: C:\Users\NANDAN~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:50155}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:50155/devtoo..., se:cdpVersion: 136.0.7103.114, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 468adb5a54026f1a1c1dbb1d5fa1d171</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ortu@2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unexpected alert open: {Alert text : Login failed. Invalid password.}
+  (Session info: chrome=136.0.7103.114): Login failed. Invalid password.
+Build info: version: '4.30.0', revision: '509c7f17cc*'
+System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '23.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Command: [05eda5f4ec412026584d58917b36a072, getCurrentUrl {}]
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 136.0.7103.114, chrome: {chromedriverVersion: 136.0.7103.94 (fa0be0b33deb..., userDataDir: C:\Users\NANDAN~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:50200}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:50200/devtoo..., se:cdpVersion: 136.0.7103.114, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 05eda5f4ec412026584d58917b36a072</t>
+  </si>
+  <si>
+    <t xml:space="preserve">orru@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gmail@2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unexpected alert open: {Alert text : Login failed. Email not found.}
+  (Session info: chrome=136.0.7103.114): Login failed. Email not found.
+Build info: version: '4.30.0', revision: '509c7f17cc*'
+System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '23.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Command: [915b9658edf3e6da56cde5a58acafc23, getCurrentUrl {}]
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 136.0.7103.114, chrome: {chromedriverVersion: 136.0.7103.94 (fa0be0b33deb..., userDataDir: C:\Users\NANDAN~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:50229}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:50229/devtoo..., se:cdpVersion: 136.0.7103.114, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 915b9658edf3e6da56cde5a58acafc23</t>
   </si>
 </sst>
 </file>
@@ -122,7 +164,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -133,6 +175,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -152,18 +202,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="3.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="69.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="0.91"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -184,13 +235,51 @@
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="emerg@emergindia.org"/>
+    <hyperlink ref="A3" r:id="rId2" display="ortu@gmail.com"/>
+    <hyperlink ref="A4" r:id="rId3" display="emerg@emergindia.org"/>
+    <hyperlink ref="B4" r:id="rId4" display="ortu@2024"/>
+    <hyperlink ref="A5" r:id="rId5" display="orru@gmail.com"/>
+    <hyperlink ref="B5" r:id="rId6" display="gmail@2024"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -215,7 +304,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="2.58"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Have shown to Shachi ma'am regarding excel of Automation
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -9,7 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="DashboardData" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="CategoryData" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t xml:space="preserve">email</t>
   </si>
@@ -38,49 +38,22 @@
     <t xml:space="preserve">eVENKART@2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Login Successful</t>
-  </si>
-  <si>
     <t xml:space="preserve">ortu@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">unexpected alert open: {Alert text : Login failed. Email not found.}
-  (Session info: chrome=136.0.7103.114): Login failed. Email not found.
-Build info: version: '4.30.0', revision: '509c7f17cc*'
-System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '23.0.1'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Command: [468adb5a54026f1a1c1dbb1d5fa1d171, getCurrentUrl {}]
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 136.0.7103.114, chrome: {chromedriverVersion: 136.0.7103.94 (fa0be0b33deb..., userDataDir: C:\Users\NANDAN~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:50155}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:50155/devtoo..., se:cdpVersion: 136.0.7103.114, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
-Session ID: 468adb5a54026f1a1c1dbb1d5fa1d171</t>
-  </si>
-  <si>
     <t xml:space="preserve">ortu@2024</t>
   </si>
   <si>
-    <t xml:space="preserve">unexpected alert open: {Alert text : Login failed. Invalid password.}
-  (Session info: chrome=136.0.7103.114): Login failed. Invalid password.
-Build info: version: '4.30.0', revision: '509c7f17cc*'
-System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '23.0.1'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Command: [05eda5f4ec412026584d58917b36a072, getCurrentUrl {}]
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 136.0.7103.114, chrome: {chromedriverVersion: 136.0.7103.94 (fa0be0b33deb..., userDataDir: C:\Users\NANDAN~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:50200}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:50200/devtoo..., se:cdpVersion: 136.0.7103.114, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
-Session ID: 05eda5f4ec412026584d58917b36a072</t>
-  </si>
-  <si>
     <t xml:space="preserve">orru@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">gmail@2024</t>
   </si>
   <si>
-    <t xml:space="preserve">unexpected alert open: {Alert text : Login failed. Email not found.}
-  (Session info: chrome=136.0.7103.114): Login failed. Email not found.
-Build info: version: '4.30.0', revision: '509c7f17cc*'
-System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '23.0.1'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Command: [915b9658edf3e6da56cde5a58acafc23, getCurrentUrl {}]
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 136.0.7103.114, chrome: {chromedriverVersion: 136.0.7103.94 (fa0be0b33deb..., userDataDir: C:\Users\NANDAN~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:50229}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:50229/devtoo..., se:cdpVersion: 136.0.7103.114, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
-Session ID: 915b9658edf3e6da56cde5a58acafc23</t>
+    <t xml:space="preserve">Category Name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category Image</t>
   </si>
 </sst>
 </file>
@@ -205,16 +178,16 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="69.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="0.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="47.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="0.22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -235,42 +208,34 @@
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="C3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>9</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>12</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C5" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -296,17 +261,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="C2:C5 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="2.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="0.64"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Ran the testscript and it works fine till Add user
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
   <si>
     <t xml:space="preserve">email</t>
   </si>
@@ -232,6 +232,27 @@
 Command: [5d3114751f4553e96015d026789b177d, getCurrentUrl {}]
 Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 136.0.7103.114, chrome: {chromedriverVersion: 136.0.7103.113 (76fa3c17824..., userDataDir: C:\Users\NANDAN~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:61558}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:61558/devtoo..., se:cdpVersion: 136.0.7103.114, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
 Session ID: 5d3114751f4553e96015d026789b177d</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//input[@id='searchUserDetails1']//option[contains(text(),'Distributor')]"}
+  (Session info: chrome=136.0.7103.114)
+For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
+Build info: version: '4.30.0', revision: '509c7f17cc*'
+System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '23.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Command: [2ae64c9022fecb543a3b4acb53db6aa1, findElement {value=//input[@id='searchUserDetails1']//option[contains(text(),'Distributor')], using=xpath}]
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 136.0.7103.114, chrome: {chromedriverVersion: 136.0.7103.113 (76fa3c17824..., userDataDir: C:\Users\NANDAN~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:61320}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:61320/devtoo..., se:cdpVersion: 136.0.7103.114, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 2ae64c9022fecb543a3b4acb53db6aa1</t>
+  </si>
+  <si>
+    <t>unexpected alert open: {Alert text : Login failed. Email not found.}
+  (Session info: chrome=136.0.7103.114): Login failed. Email not found.
+Build info: version: '4.30.0', revision: '509c7f17cc*'
+System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '23.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Command: [5da612ce94c7b2f9efce380f9f77a8fa, getCurrentUrl {}]
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 136.0.7103.114, chrome: {chromedriverVersion: 136.0.7103.113 (76fa3c17824..., userDataDir: C:\Users\NANDAN~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:61741}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:61741/devtoo..., se:cdpVersion: 136.0.7103.114, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 5da612ce94c7b2f9efce380f9f77a8fa</t>
   </si>
 </sst>
 </file>
@@ -387,7 +408,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -398,7 +419,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Admin script completed fully but working on excel
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation\My Workspace (Selenium)\Selenium Web Driver\OrtusolisAutomationProject\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E2A180-3682-4C02-86AF-40FBA02A0E25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9420C610-EB13-4428-8DE7-BAB377BABC8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="SubCategory" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
   <si>
     <t>email</t>
   </si>
@@ -62,242 +63,44 @@
     <t>Category Image</t>
   </si>
   <si>
-    <t>Login Successful</t>
-  </si>
-  <si>
-    <t>invalid session id: session deleted as the browser has closed the connection
-from disconnected: not connected to DevTools
-  (Session info: chrome=137.0.7151.41)
-Build info: version: '4.30.0', revision: '509c7f17cc*'
-System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '21.0.6'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Command: [07616bdae644ce2d7d69fb078470bf91, findElement {using=id, value=search_input_all}]
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 137.0.7151.41, chrome: {chromedriverVersion: 137.0.7151.40 (84781974514a..., userDataDir: C:\Users\nanda\AppData\Loca...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:60205}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:60205/devtoo..., se:cdpVersion: 137.0.7151.41, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
-Session ID: 07616bdae644ce2d7d69fb078470bf91</t>
-  </si>
-  <si>
-    <t>element not interactable
-  (Session info: chrome=137.0.7151.41)
-Build info: version: '4.30.0', revision: '509c7f17cc*'
-System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '21.0.6'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Command: [413fc01d3d3dae257b985eeca2a3b972, clickElement {id=f.CE818DF888CBE2827DEE86F70B1B3184.d.5993C1642FBE231F1045C2B6D23D45F9.e.1763}]
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 137.0.7151.41, chrome: {chromedriverVersion: 137.0.7151.40 (84781974514a..., userDataDir: C:\Users\nanda\AppData\Loca...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:60974}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:60974/devtoo..., se:cdpVersion: 137.0.7151.41, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
-Element: [[ChromeDriver: chrome on windows (413fc01d3d3dae257b985eeca2a3b972)] -&gt; xpath: //tbody/tr[39]/td[4]/div[1]/button[1]]
-Session ID: 413fc01d3d3dae257b985eeca2a3b972</t>
-  </si>
-  <si>
-    <t>unexpected alert open: {Alert text : Login failed. Email not found.}
-  (Session info: chrome=137.0.7151.41): Login failed. Email not found.
-Build info: version: '4.30.0', revision: '509c7f17cc*'
-System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '21.0.6'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Command: [0ccd6cf8568e2a5245a4a3f490addc1e, getCurrentUrl {}]
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 137.0.7151.41, chrome: {chromedriverVersion: 137.0.7151.40 (84781974514a..., userDataDir: C:\Users\nanda\AppData\Loca...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:61220}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:61220/devtoo..., se:cdpVersion: 137.0.7151.41, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
-Session ID: 0ccd6cf8568e2a5245a4a3f490addc1e</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//input[@id='searchUserDetails1']//option[contains(text(),'Distributor')]"}
-  (Session info: chrome=137.0.7151.41)
-For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
-Build info: version: '4.30.0', revision: '509c7f17cc*'
-System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '21.0.6'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Command: [4fbfcca18437ffb283ccbfe5840febf3, findElement {using=xpath, value=//input[@id='searchUserDetails1']//option[contains(text(),'Distributor')]}]
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 137.0.7151.41, chrome: {chromedriverVersion: 137.0.7151.40 (84781974514a..., userDataDir: C:\Users\nanda\AppData\Loca...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:61728}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:61728/devtoo..., se:cdpVersion: 137.0.7151.41, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
-Session ID: 4fbfcca18437ffb283ccbfe5840febf3</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//select[@id='attributecategory']//option[contains(text(),'Testing Category')]"}
-  (Session info: chrome=137.0.7151.41)
-For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
-Build info: version: '4.30.0', revision: '509c7f17cc*'
-System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '21.0.6'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Command: [e6948604f0f5f19f2685c036c3171444, findElement {using=xpath, value=//select[@id='attributecategory']//option[contains(text(),'Testing Category')]}]
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 137.0.7151.41, chrome: {chromedriverVersion: 137.0.7151.40 (84781974514a..., userDataDir: C:\Users\nanda\AppData\Loca...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:61873}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:61873/devtoo..., se:cdpVersion: 137.0.7151.41, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
-Session ID: e6948604f0f5f19f2685c036c3171444</t>
-  </si>
-  <si>
-    <t>unexpected alert open: {Alert text : Login failed. Email not found.}
-  (Session info: chrome=137.0.7151.41): Login failed. Email not found.
-Build info: version: '4.30.0', revision: '509c7f17cc*'
-System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '21.0.6'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Command: [aee11cc29419c2160137863759a4772f, getCurrentUrl {}]
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 137.0.7151.41, chrome: {chromedriverVersion: 137.0.7151.40 (84781974514a..., userDataDir: C:\Users\nanda\AppData\Loca...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:62159}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:62159/devtoo..., se:cdpVersion: 137.0.7151.41, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
-Session ID: aee11cc29419c2160137863759a4772f</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//button[normalize-space()='Delete']"}
-  (Session info: chrome=137.0.7151.41)
-For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
-Build info: version: '4.30.0', revision: '509c7f17cc*'
-System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '21.0.6'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Command: [03e06b9d941b90e9048a51b998592930, findElement {using=xpath, value=//button[normalize-space()='Delete']}]
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 137.0.7151.41, chrome: {chromedriverVersion: 137.0.7151.40 (84781974514a..., userDataDir: C:\Users\nanda\AppData\Loca...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:62207}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:62207/devtoo..., se:cdpVersion: 137.0.7151.41, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
-Session ID: 03e06b9d941b90e9048a51b998592930</t>
-  </si>
-  <si>
-    <t>unexpected alert open: {Alert text : Login failed. Email not found.}
-  (Session info: chrome=137.0.7151.41): Login failed. Email not found.
-Build info: version: '4.30.0', revision: '509c7f17cc*'
-System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '21.0.6'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Command: [33bfa939620a2f2c9e785baef3d9a51a, getCurrentUrl {}]
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 137.0.7151.41, chrome: {chromedriverVersion: 137.0.7151.40 (84781974514a..., userDataDir: C:\Users\nanda\AppData\Loca...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:62554}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:62554/devtoo..., se:cdpVersion: 137.0.7151.41, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
-Session ID: 33bfa939620a2f2c9e785baef3d9a51a</t>
-  </si>
-  <si>
-    <t>element not interactable
-  (Session info: chrome=137.0.7151.41)
-Build info: version: '4.30.0', revision: '509c7f17cc*'
-System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '21.0.6'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Command: [ace6ea7d97eadb3446da68dae4962a12, clickElement {id=f.92788A8D577ABEFD949304C0AFC2B715.d.5B1A0736A0E5244ADB28161FD92F9282.e.1769}]
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 137.0.7151.41, chrome: {chromedriverVersion: 137.0.7151.40 (84781974514a..., userDataDir: C:\Users\nanda\AppData\Loca...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:62706}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:62706/devtoo..., se:cdpVersion: 137.0.7151.41, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
-Element: [[ChromeDriver: chrome on windows (ace6ea7d97eadb3446da68dae4962a12)] -&gt; xpath: //tbody/tr[39]/td[4]/div[1]/button[1]]
-Session ID: ace6ea7d97eadb3446da68dae4962a12</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//input[@id='searchUserDetails1']//option[contains(text(),'Distributor')]"}
-  (Session info: chrome=137.0.7151.41)
-For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
-Build info: version: '4.30.0', revision: '509c7f17cc*'
-System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '21.0.6'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Command: [1b83496bf8779066f43d5dbbd9f2cfb2, findElement {value=//input[@id='searchUserDetails1']//option[contains(text(),'Distributor')], using=xpath}]
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 137.0.7151.41, chrome: {chromedriverVersion: 137.0.7151.40 (84781974514a..., userDataDir: C:\Users\nanda\AppData\Loca...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:63053}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:63053/devtoo..., se:cdpVersion: 137.0.7151.41, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
-Session ID: 1b83496bf8779066f43d5dbbd9f2cfb2</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//select[@id='attributecategory']//option[contains(text(),'Testing Category')]"}
-  (Session info: chrome=137.0.7151.41)
-For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
-Build info: version: '4.30.0', revision: '509c7f17cc*'
-System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '21.0.6'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Command: [c9e517c5dc12a6c5c32a8e6202b097da, findElement {using=xpath, value=//select[@id='attributecategory']//option[contains(text(),'Testing Category')]}]
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 137.0.7151.41, chrome: {chromedriverVersion: 137.0.7151.40 (84781974514a..., userDataDir: C:\Users\nanda\AppData\Loca...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:63426}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:63426/devtoo..., se:cdpVersion: 137.0.7151.41, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
-Session ID: c9e517c5dc12a6c5c32a8e6202b097da</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//*[@name='categories']//option[contains(text(),'Astra Designs')]"}
-  (Session info: chrome=137.0.7151.41)
-For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
-Build info: version: '4.30.0', revision: '509c7f17cc*'
-System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '21.0.6'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Command: [e2f713d8eb4c1220ef17fcf94d8eeb9f, findElement {using=xpath, value=//*[@name='categories']//option[contains(text(),'Astra Designs')]}]
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 137.0.7151.41, chrome: {chromedriverVersion: 137.0.7151.40 (84781974514a..., userDataDir: C:\Users\nanda\AppData\Loca...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:63805}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:63805/devtoo..., se:cdpVersion: 137.0.7151.41, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
-Session ID: e2f713d8eb4c1220ef17fcf94d8eeb9f</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//input[@id='searchUserDetails1']//option[contains(text(),'Distributor')]"}
-  (Session info: chrome=137.0.7151.41)
-For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
-Build info: version: '4.30.0', revision: '509c7f17cc*'
-System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '21.0.6'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Command: [37281ff92e1b2afa6eec002b8fe9abc0, findElement {value=//input[@id='searchUserDetails1']//option[contains(text(),'Distributor')], using=xpath}]
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 137.0.7151.41, chrome: {chromedriverVersion: 137.0.7151.40 (84781974514a..., userDataDir: C:\Users\nanda\AppData\Loca...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:63887}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:63887/devtoo..., se:cdpVersion: 137.0.7151.41, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
-Session ID: 37281ff92e1b2afa6eec002b8fe9abc0</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//input[@id='searchUserDetails1']//option[contains(text(),'Distributor')]"}
-  (Session info: chrome=137.0.7151.41)
-For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
-Build info: version: '4.30.0', revision: '509c7f17cc*'
-System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '21.0.6'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Command: [c500026221d65e96b159981eefeb61c8, findElement {using=xpath, value=//input[@id='searchUserDetails1']//option[contains(text(),'Distributor')]}]
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 137.0.7151.41, chrome: {chromedriverVersion: 137.0.7151.40 (84781974514a..., userDataDir: C:\Users\nanda\AppData\Loca...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:64304}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:64304/devtoo..., se:cdpVersion: 137.0.7151.41, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
-Session ID: c500026221d65e96b159981eefeb61c8</t>
-  </si>
-  <si>
-    <t>element not interactable
-  (Session info: chrome=137.0.7151.41)
-Build info: version: '4.30.0', revision: '509c7f17cc*'
-System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '21.0.6'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Command: [376657bae328f39afab159879b58a05b, clickElement {id=f.CC3AEB8258A57123D7CB064E21C739CE.d.397E059AF35C2CCF6CF5BE42F287619F.e.2345}]
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 137.0.7151.41, chrome: {chromedriverVersion: 137.0.7151.40 (84781974514a..., userDataDir: C:\Users\nanda\AppData\Loca...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:64836}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:64836/devtoo..., se:cdpVersion: 137.0.7151.41, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
-Element: [[ChromeDriver: chrome on windows (376657bae328f39afab159879b58a05b)] -&gt; xpath: //tbody/tr[1]/td[8]/div[1]/button[2]]
-Session ID: 376657bae328f39afab159879b58a05b</t>
-  </si>
-  <si>
-    <t>unexpected alert open: {Alert text : Login failed. Email not found.}
-  (Session info: chrome=137.0.7151.41): Login failed. Email not found.
-Build info: version: '4.30.0', revision: '509c7f17cc*'
-System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '21.0.6'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Command: [ff2aeb487d7775e514fec728bbcb4445, getCurrentUrl {}]
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 137.0.7151.41, chrome: {chromedriverVersion: 137.0.7151.40 (84781974514a..., userDataDir: C:\Users\nanda\AppData\Loca...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:65318}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:65318/devtoo..., se:cdpVersion: 137.0.7151.41, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
-Session ID: ff2aeb487d7775e514fec728bbcb4445</t>
-  </si>
-  <si>
-    <t>no such window: target window already closed
-from unknown error: web view not found
-  (Session info: chrome=137.0.7151.41)
-Build info: version: '4.30.0', revision: '509c7f17cc*'
-System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '21.0.6'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Command: [fd4d7bf1499690847d9a43718a7f6153, getCurrentUrl {}]
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 137.0.7151.41, chrome: {chromedriverVersion: 137.0.7151.40 (84781974514a..., userDataDir: C:\Users\nanda\AppData\Loca...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:65344}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:65344/devtoo..., se:cdpVersion: 137.0.7151.41, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
-Session ID: fd4d7bf1499690847d9a43718a7f6153</t>
-  </si>
-  <si>
-    <t>unexpected alert open: {Alert text : Login failed. Invalid password.}
-  (Session info: chrome=137.0.7151.41): Login failed. Invalid password.
-Build info: version: '4.30.0', revision: '509c7f17cc*'
-System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '21.0.6'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Command: [38c2c78a56db74436c25a7d41a782934, getCurrentUrl {}]
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 137.0.7151.41, chrome: {chromedriverVersion: 137.0.7151.55 (254bc711794d..., userDataDir: C:\Users\nanda\AppData\Loca...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:52843}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:52843/devtoo..., se:cdpVersion: 137.0.7151.41, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
-Session ID: 38c2c78a56db74436c25a7d41a782934</t>
-  </si>
-  <si>
-    <t>unexpected alert open: {Alert text : Login failed. Email not found.}
-  (Session info: chrome=137.0.7151.41): Login failed. Email not found.
-Build info: version: '4.30.0', revision: '509c7f17cc*'
-System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '21.0.6'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Command: [8b59c5744b85ac070664c1893b66ef37, getCurrentUrl {}]
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 137.0.7151.41, chrome: {chromedriverVersion: 137.0.7151.55 (254bc711794d..., userDataDir: C:\Users\nanda\AppData\Loca...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:52865}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:52865/devtoo..., se:cdpVersion: 137.0.7151.41, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
-Session ID: 8b59c5744b85ac070664c1893b66ef37</t>
-  </si>
-  <si>
-    <t>unexpected alert open: {Alert text : Login failed. Email not found.}
-  (Session info: chrome=137.0.7151.41): Login failed. Email not found.
-Build info: version: '4.30.0', revision: '509c7f17cc*'
-System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '21.0.6'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Command: [384b6898b533eef6515c4592c5bae8b4, getCurrentUrl {}]
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 137.0.7151.41, chrome: {chromedriverVersion: 137.0.7151.55 (254bc711794d..., userDataDir: C:\Users\nanda\AppData\Loca...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:53586}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:53586/devtoo..., se:cdpVersion: 137.0.7151.41, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
-Session ID: 384b6898b533eef6515c4592c5bae8b4</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//button[normalize-space()='Yes, Delete']"}
-  (Session info: chrome=137.0.7151.41)
-For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
-Build info: version: '4.30.0', revision: '509c7f17cc*'
-System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '21.0.6'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Command: [96663e5cb5a772cc257e9b725aceb8d6, findElement {using=xpath, value=//button[normalize-space()='Yes, Delete']}]
-Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 137.0.7151.41, chrome: {chromedriverVersion: 137.0.7151.55 (254bc711794d..., userDataDir: C:\Users\nanda\AppData\Loca...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:53616}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:53616/devtoo..., se:cdpVersion: 137.0.7151.41, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
-Session ID: 96663e5cb5a772cc257e9b725aceb8d6</t>
-  </si>
-  <si>
-    <t>Expected condition failed: waiting for presence of element located by: By.xpath: //table[@id='ordertable']//td (tried for 15 second(s) with 500 milliseconds interval)</t>
+    <t>Add Category</t>
+  </si>
+  <si>
+    <t>Nutrional Flag</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>C:\Users\nanda\Downloads\imageb.jpg</t>
+  </si>
+  <si>
+    <t>Select Category</t>
+  </si>
+  <si>
+    <t>Sub-Category image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing Category </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adding Sub </t>
+  </si>
+  <si>
+    <t>"C:\Users\nanda\Downloads\imageb (1).jpg"</t>
+  </si>
+  <si>
+    <t>Sub-Category Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -310,6 +113,17 @@
       <color rgb="FF000000"/>
       <name val="Roboto"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="2">
@@ -334,7 +148,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
@@ -346,6 +160,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -683,17 +506,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="24.0"/>
-    <col min="2" max="2" customWidth="true" width="38.8984375"/>
-    <col min="3" max="3" customWidth="true" width="50.3984375"/>
-    <col min="4" max="4" customWidth="true" width="3.69921875"/>
-    <col min="5" max="1025" customWidth="true" width="0.09765625"/>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="2" width="38.8984375" customWidth="1"/>
+    <col min="3" max="3" width="50.3984375" customWidth="1"/>
+    <col min="4" max="4" width="3.69921875" customWidth="1"/>
+    <col min="5" max="1025" width="9.765625E-2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -714,42 +537,34 @@
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>33</v>
-      </c>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>31</v>
-      </c>
+      <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="C5" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -767,34 +582,85 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="12.8984375"/>
-    <col min="2" max="2" customWidth="true" width="17.296875"/>
-    <col min="3" max="3" customWidth="true" width="34.8984375"/>
-    <col min="4" max="1025" customWidth="true" width="0.296875"/>
+    <col min="1" max="1" width="12.8984375" customWidth="1"/>
+    <col min="2" max="2" width="65" customWidth="1"/>
+    <col min="3" max="3" width="58.69921875" customWidth="1"/>
+    <col min="4" max="4" width="34.8984375" customWidth="1"/>
+    <col min="5" max="1026" width="0.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -804,14 +670,88 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE0054AC-08BE-4830-B0A0-05A528F13DD0}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="25.19921875" customWidth="1"/>
+    <col min="2" max="2" width="22.8984375" customWidth="1"/>
+    <col min="3" max="3" width="45.09765625" customWidth="1"/>
+    <col min="4" max="4" width="20.3984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>